<commit_message>
feat: Actualizar LinkedIn y foto de Angelo Moreno y Manuel Bazaes
- Angelo Moreno: agregar foto real y LinkedIn actualizado
- Manuel Bazaes: actualizar LinkedIn
- Instalar dependencia critters faltante
</commit_message>
<xml_diff>
--- a/docs/Quiero saber cómo te sentiste trabajando conmigo  (Respuestas).xlsx
+++ b/docs/Quiero saber cómo te sentiste trabajando conmigo  (Respuestas).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcasanovam/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcasanovam/www/hugotech/hugotech_landing_web/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F855BB-B4C5-8245-903C-53F921DB9E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F776E8A3-B9CF-3E46-BBB5-1FEE10BA95E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="620" windowWidth="38400" windowHeight="20980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respuestas de formulario 1" sheetId="1" r:id="rId1"/>
@@ -881,9 +881,9 @@
   </sheetPr>
   <dimension ref="A1:L131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1497,7 +1497,7 @@
         <v>19</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="K16" s="5" t="s">
         <v>89</v>
@@ -1535,7 +1535,7 @@
         <v>28</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="K17" s="5" t="s">
         <v>94</v>

</xml_diff>